<commit_message>
simlutate type/click instead of hardware events
</commit_message>
<xml_diff>
--- a/Data Entry Automation/BankData.xlsx
+++ b/Data Entry Automation/BankData.xlsx
@@ -55,97 +55,97 @@
     <x:t>Cheque</x:t>
   </x:si>
   <x:si>
-    <x:t>205447</x:t>
-  </x:si>
-  <x:si>
-    <x:t>676566</x:t>
-  </x:si>
-  <x:si>
-    <x:t>717868</x:t>
+    <x:t>523788</x:t>
+  </x:si>
+  <x:si>
+    <x:t>630822</x:t>
+  </x:si>
+  <x:si>
+    <x:t>414931</x:t>
   </x:si>
   <x:si>
     <x:t>Cash</x:t>
   </x:si>
   <x:si>
-    <x:t>611913</x:t>
-  </x:si>
-  <x:si>
-    <x:t>183033</x:t>
-  </x:si>
-  <x:si>
-    <x:t>654151</x:t>
-  </x:si>
-  <x:si>
-    <x:t>871120</x:t>
-  </x:si>
-  <x:si>
-    <x:t>765164</x:t>
-  </x:si>
-  <x:si>
-    <x:t>336284</x:t>
-  </x:si>
-  <x:si>
-    <x:t>876176</x:t>
-  </x:si>
-  <x:si>
-    <x:t>447296</x:t>
-  </x:si>
-  <x:si>
-    <x:t>517006</x:t>
-  </x:si>
-  <x:si>
-    <x:t>411051</x:t>
-  </x:si>
-  <x:si>
-    <x:t>305095</x:t>
-  </x:si>
-  <x:si>
-    <x:t>522063</x:t>
-  </x:si>
-  <x:si>
-    <x:t>591773</x:t>
-  </x:si>
-  <x:si>
-    <x:t>407333</x:t>
-  </x:si>
-  <x:si>
-    <x:t>154119</x:t>
-  </x:si>
-  <x:si>
-    <x:t>546753</x:t>
-  </x:si>
-  <x:si>
-    <x:t>588055</x:t>
-  </x:si>
-  <x:si>
-    <x:t>334841</x:t>
-  </x:si>
-  <x:si>
-    <x:t>727476</x:t>
-  </x:si>
-  <x:si>
-    <x:t>944444</x:t>
-  </x:si>
-  <x:si>
-    <x:t>114155</x:t>
-  </x:si>
-  <x:si>
-    <x:t>183865</x:t>
-  </x:si>
-  <x:si>
-    <x:t>576500</x:t>
-  </x:si>
-  <x:si>
-    <x:t>793468</x:t>
-  </x:si>
-  <x:si>
-    <x:t>637435</x:t>
-  </x:si>
-  <x:si>
-    <x:t>854404</x:t>
-  </x:si>
-  <x:si>
-    <x:t>924114</x:t>
+    <x:t>647554</x:t>
+  </x:si>
+  <x:si>
+    <x:t>704511</x:t>
+  </x:si>
+  <x:si>
+    <x:t>438543</x:t>
+  </x:si>
+  <x:si>
+    <x:t>319834</x:t>
+  </x:si>
+  <x:si>
+    <x:t>376791</x:t>
+  </x:si>
+  <x:si>
+    <x:t>982415</x:t>
+  </x:si>
+  <x:si>
+    <x:t>139373</x:t>
+  </x:si>
+  <x:si>
+    <x:t>676223</x:t>
+  </x:si>
+  <x:si>
+    <x:t>607590</x:t>
+  </x:si>
+  <x:si>
+    <x:t>244442</x:t>
+  </x:si>
+  <x:si>
+    <x:t>928550</x:t>
+  </x:si>
+  <x:si>
+    <x:t>584098</x:t>
+  </x:si>
+  <x:si>
+    <x:t>239646</x:t>
+  </x:si>
+  <x:si>
+    <x:t>873678</x:t>
+  </x:si>
+  <x:si>
+    <x:t>353560</x:t>
+  </x:si>
+  <x:si>
+    <x:t>410517</x:t>
+  </x:si>
+  <x:si>
+    <x:t>370292</x:t>
+  </x:si>
+  <x:si>
+    <x:t>301659</x:t>
+  </x:si>
+  <x:si>
+    <x:t>211358</x:t>
+  </x:si>
+  <x:si>
+    <x:t>318392</x:t>
+  </x:si>
+  <x:si>
+    <x:t>102501</x:t>
+  </x:si>
+  <x:si>
+    <x:t>385201</x:t>
+  </x:si>
+  <x:si>
+    <x:t>843566</x:t>
+  </x:si>
+  <x:si>
+    <x:t>452009</x:t>
+  </x:si>
+  <x:si>
+    <x:t>236119</x:t>
+  </x:si>
+  <x:si>
+    <x:t>920227</x:t>
+  </x:si>
+  <x:si>
+    <x:t>654260</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -209,9 +209,24 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="7">
+  <x:cellStyleXfs count="12">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">

</xml_diff>